<commit_message>
Fixing class initialization problems...
</commit_message>
<xml_diff>
--- a/analyzer/results/references/finals.xlsx
+++ b/analyzer/results/references/finals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59961D1F-D5F9-4C00-8063-1108C7CD152D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC68D0BD-BD46-4F67-B613-E5CEAD7B62E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="392">
   <si>
     <t>Owner</t>
   </si>
@@ -1153,9 +1153,6 @@
     <t>Effectively immutable</t>
   </si>
   <si>
-    <t>Collection never returned</t>
-  </si>
-  <si>
     <t>Immutable components</t>
   </si>
   <si>
@@ -1168,10 +1165,46 @@
     <t>Requires change in source code</t>
   </si>
   <si>
-    <t>Note 1</t>
-  </si>
-  <si>
-    <t>Note 2</t>
+    <t>Never modified</t>
+  </si>
+  <si>
+    <t>IllegalAccessException or IllegalCallerException can be thrown</t>
+  </si>
+  <si>
+    <t>Field type is not immutable but the assigned values to the final field are immutable</t>
+  </si>
+  <si>
+    <t>Never returned to tenant modules</t>
+  </si>
+  <si>
+    <t>For instance, the type is not a final class and can be subclassed but it is not subclassed in java.base and not exported to tenant modules</t>
+  </si>
+  <si>
+    <t>Cannot be modified by tenant modules</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>This shouldn't be used</t>
+  </si>
+  <si>
+    <t>ThreadLocal</t>
+  </si>
+  <si>
+    <t>Since each thread belongs to one and only one tenant at any given time, changes in static ThreadLocal variables do not violate tenant-isolation requirements</t>
+  </si>
+  <si>
+    <t>Never returned</t>
+  </si>
+  <si>
+    <t>For instance, for enforcing permission checks and/or adding privileged blocks</t>
+  </si>
+  <si>
+    <t>Component</t>
   </si>
 </sst>
 </file>
@@ -1491,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,6 +1533,8 @@
     <col min="1" max="1" width="47.140625" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
     <col min="3" max="3" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,10 +1548,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,6 +1564,9 @@
       <c r="C2" t="s">
         <v>125</v>
       </c>
+      <c r="D2" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1540,6 +1578,9 @@
       <c r="C3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1551,6 +1592,9 @@
       <c r="C4" t="s">
         <v>68</v>
       </c>
+      <c r="D4" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1562,6 +1606,9 @@
       <c r="C5" t="s">
         <v>68</v>
       </c>
+      <c r="D5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1573,6 +1620,9 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
+      <c r="D6" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1584,6 +1634,9 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
+      <c r="D7" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1595,6 +1648,9 @@
       <c r="C8" t="s">
         <v>61</v>
       </c>
+      <c r="D8" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1606,6 +1662,9 @@
       <c r="C9" t="s">
         <v>61</v>
       </c>
+      <c r="D9" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1617,6 +1676,9 @@
       <c r="C10" t="s">
         <v>173</v>
       </c>
+      <c r="D10" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1628,6 +1690,9 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
+      <c r="D11" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1639,6 +1704,9 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
+      <c r="D12" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1650,6 +1718,9 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
+      <c r="D13" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1661,6 +1732,9 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
+      <c r="D14" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1672,6 +1746,9 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
+      <c r="D15" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1683,8 +1760,11 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1694,8 +1774,11 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -1705,8 +1788,11 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -1716,8 +1802,11 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>168</v>
       </c>
@@ -1727,8 +1816,11 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -1738,8 +1830,11 @@
       <c r="C21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>216</v>
       </c>
@@ -1749,8 +1844,11 @@
       <c r="C22" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1760,8 +1858,14 @@
       <c r="C23" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>381</v>
+      </c>
+      <c r="E23" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -1771,8 +1875,14 @@
       <c r="C24" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>381</v>
+      </c>
+      <c r="E24" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1782,8 +1892,11 @@
       <c r="C25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1793,8 +1906,11 @@
       <c r="C26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -1804,8 +1920,11 @@
       <c r="C27" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1815,8 +1934,11 @@
       <c r="C28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1826,8 +1948,11 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1837,8 +1962,11 @@
       <c r="C30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>214</v>
       </c>
@@ -1848,8 +1976,11 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -1859,8 +1990,11 @@
       <c r="C32" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -1870,8 +2004,11 @@
       <c r="C33" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1881,8 +2018,11 @@
       <c r="C34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>204</v>
       </c>
@@ -1892,8 +2032,11 @@
       <c r="C35" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1903,8 +2046,11 @@
       <c r="C36" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1914,8 +2060,11 @@
       <c r="C37" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1925,8 +2074,11 @@
       <c r="C38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1936,8 +2088,11 @@
       <c r="C39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1947,8 +2102,11 @@
       <c r="C40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1958,8 +2116,11 @@
       <c r="C41" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1969,8 +2130,11 @@
       <c r="C42" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>148</v>
       </c>
@@ -1980,8 +2144,11 @@
       <c r="C43" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1991,8 +2158,11 @@
       <c r="C44" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -2002,8 +2172,11 @@
       <c r="C45" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -2013,8 +2186,14 @@
       <c r="C46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>377</v>
+      </c>
+      <c r="E46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -2024,8 +2203,14 @@
       <c r="C47" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>377</v>
+      </c>
+      <c r="E47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2035,8 +2220,14 @@
       <c r="C48" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>375</v>
+      </c>
+      <c r="E48" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -2046,8 +2237,14 @@
       <c r="C49" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>377</v>
+      </c>
+      <c r="E49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2057,8 +2254,14 @@
       <c r="C50" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>377</v>
+      </c>
+      <c r="E50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -2069,7 +2272,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -2079,8 +2282,11 @@
       <c r="C52" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>117</v>
       </c>
@@ -2090,8 +2296,14 @@
       <c r="C53" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>373</v>
+      </c>
+      <c r="E53" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -2101,8 +2313,14 @@
       <c r="C54" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>373</v>
+      </c>
+      <c r="E54" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -2112,8 +2330,14 @@
       <c r="C55" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>389</v>
+      </c>
+      <c r="E55" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2123,8 +2347,14 @@
       <c r="C56" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>373</v>
+      </c>
+      <c r="E56" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -2134,8 +2364,14 @@
       <c r="C57" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>373</v>
+      </c>
+      <c r="E57" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2145,8 +2381,14 @@
       <c r="C58" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>373</v>
+      </c>
+      <c r="E58" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2156,8 +2398,11 @@
       <c r="C59" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -2167,8 +2412,14 @@
       <c r="C60" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>378</v>
+      </c>
+      <c r="E60" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -2178,8 +2429,14 @@
       <c r="C61" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>378</v>
+      </c>
+      <c r="E61" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2189,8 +2446,14 @@
       <c r="C62" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>373</v>
+      </c>
+      <c r="E62" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -2200,8 +2463,14 @@
       <c r="C63" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>378</v>
+      </c>
+      <c r="E63" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -2211,8 +2480,14 @@
       <c r="C64" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>378</v>
+      </c>
+      <c r="E64" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -2222,8 +2497,14 @@
       <c r="C65" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>378</v>
+      </c>
+      <c r="E65" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -2233,8 +2514,14 @@
       <c r="C66" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>389</v>
+      </c>
+      <c r="E66" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -2244,8 +2531,14 @@
       <c r="C67" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>389</v>
+      </c>
+      <c r="E67" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2255,8 +2548,11 @@
       <c r="C68" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2266,8 +2562,11 @@
       <c r="C69" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>213</v>
       </c>
@@ -2277,8 +2576,11 @@
       <c r="C70" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>187</v>
       </c>
@@ -2288,8 +2590,11 @@
       <c r="C71" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -2299,8 +2604,11 @@
       <c r="C72" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -2310,8 +2618,11 @@
       <c r="C73" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -2321,8 +2632,11 @@
       <c r="C74" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -2332,8 +2646,11 @@
       <c r="C75" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>61</v>
       </c>
@@ -2343,8 +2660,14 @@
       <c r="C76" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>373</v>
+      </c>
+      <c r="E76" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>61</v>
       </c>
@@ -2354,8 +2677,14 @@
       <c r="C77" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>373</v>
+      </c>
+      <c r="E77" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -2365,8 +2694,14 @@
       <c r="C78" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>375</v>
+      </c>
+      <c r="E78" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2376,8 +2711,14 @@
       <c r="C79" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>373</v>
+      </c>
+      <c r="E79" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2387,8 +2728,14 @@
       <c r="C80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>373</v>
+      </c>
+      <c r="E80" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>120</v>
       </c>
@@ -2398,8 +2745,14 @@
       <c r="C81" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>373</v>
+      </c>
+      <c r="E81" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -2409,8 +2762,11 @@
       <c r="C82" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>93</v>
       </c>
@@ -2420,8 +2776,11 @@
       <c r="C83" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -2431,8 +2790,11 @@
       <c r="C84" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -2442,8 +2804,11 @@
       <c r="C85" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>137</v>
       </c>
@@ -2453,8 +2818,11 @@
       <c r="C86" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -2464,8 +2832,11 @@
       <c r="C87" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -2475,8 +2846,11 @@
       <c r="C88" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>145</v>
       </c>
@@ -2486,8 +2860,11 @@
       <c r="C89" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -2497,8 +2874,11 @@
       <c r="C90" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>71</v>
       </c>
@@ -2508,8 +2888,11 @@
       <c r="C91" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -2519,8 +2902,11 @@
       <c r="C92" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2530,8 +2916,11 @@
       <c r="C93" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>148</v>
       </c>
@@ -2541,8 +2930,11 @@
       <c r="C94" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -2552,8 +2944,11 @@
       <c r="C95" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>86</v>
       </c>
@@ -2563,8 +2958,11 @@
       <c r="C96" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -2574,8 +2972,11 @@
       <c r="C97" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -2585,8 +2986,11 @@
       <c r="C98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -2596,8 +3000,11 @@
       <c r="C99" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -2607,8 +3014,11 @@
       <c r="C100" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -2618,8 +3028,11 @@
       <c r="C101" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>164</v>
       </c>
@@ -2629,8 +3042,11 @@
       <c r="C102" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>31</v>
       </c>
@@ -2640,8 +3056,11 @@
       <c r="C103" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>130</v>
       </c>
@@ -2651,8 +3070,11 @@
       <c r="C104" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>163</v>
       </c>
@@ -2662,8 +3084,11 @@
       <c r="C105" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -2673,8 +3098,11 @@
       <c r="C106" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>70</v>
       </c>
@@ -2684,8 +3112,11 @@
       <c r="C107" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -2695,8 +3126,11 @@
       <c r="C108" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>131</v>
       </c>
@@ -2706,8 +3140,11 @@
       <c r="C109" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>127</v>
       </c>
@@ -2717,8 +3154,11 @@
       <c r="C110" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>41</v>
       </c>
@@ -2728,8 +3168,11 @@
       <c r="C111" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>219</v>
       </c>
@@ -2739,8 +3182,11 @@
       <c r="C112" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>155</v>
       </c>
@@ -2750,8 +3196,11 @@
       <c r="C113" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -2761,8 +3210,11 @@
       <c r="C114" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -2772,8 +3224,11 @@
       <c r="C115" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>51</v>
       </c>
@@ -2783,8 +3238,11 @@
       <c r="C116" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>51</v>
       </c>
@@ -2794,8 +3252,11 @@
       <c r="C117" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>81</v>
       </c>
@@ -2805,8 +3266,11 @@
       <c r="C118" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>81</v>
       </c>
@@ -2816,8 +3280,11 @@
       <c r="C119" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>28</v>
       </c>
@@ -2827,8 +3294,11 @@
       <c r="C120" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>56</v>
       </c>
@@ -2837,6 +3307,9 @@
       </c>
       <c r="C121" t="s">
         <v>58</v>
+      </c>
+      <c r="D121" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -2847,12 +3320,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF6BABD1-A540-4C4E-B17D-ADDB27355019}">
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E121</xm:sqref>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A7D80AD-B76D-4F4E-808A-082975E23528}">
+          <x14:formula1>
+            <xm:f>reasons!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D21 D25:D27 D29:D40 D68:D120</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88E6E823-CE9D-4823-8F74-575665822849}">
+          <x14:formula1>
+            <xm:f>reasons!$A$1:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D121:E121 E2:E21 D22:E24 D28 E25:E120 D41:D67</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2862,10 +3347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B8F82B-5713-437A-A243-34ABFB350BC5}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,9 +3358,11 @@
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2885,8 +3372,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -2896,8 +3389,14 @@
       <c r="C2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>231</v>
       </c>
@@ -2908,7 +3407,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>256</v>
       </c>
@@ -2919,7 +3418,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -2930,7 +3429,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2941,7 +3440,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -2952,7 +3451,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -2963,7 +3462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2974,7 +3473,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -2984,8 +3483,11 @@
       <c r="C10" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -2996,7 +3498,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -3007,7 +3509,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>228</v>
       </c>
@@ -3018,7 +3520,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>242</v>
       </c>
@@ -3029,7 +3531,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -3039,8 +3541,11 @@
       <c r="C15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>237</v>
       </c>
@@ -3050,8 +3555,11 @@
       <c r="C16" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>241</v>
       </c>
@@ -3061,8 +3569,11 @@
       <c r="C17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -3071,6 +3582,9 @@
       </c>
       <c r="C18" t="s">
         <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3079,6 +3593,18 @@
     <sortCondition ref="A3:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{833336D6-9F11-4C96-976C-F2A59342F598}">
+          <x14:formula1>
+            <xm:f>reasons!$A$1:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:E18</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3098,9 +3624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3600B5-2A22-43DF-8B3A-881817398BDB}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85:E87"/>
-    </sheetView>
+    <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3122,10 +3646,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="E1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,7 +3663,7 @@
         <v>303</v>
       </c>
       <c r="D2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3153,7 +3677,7 @@
         <v>303</v>
       </c>
       <c r="D3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3167,7 +3691,7 @@
         <v>303</v>
       </c>
       <c r="D4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3181,7 +3705,7 @@
         <v>344</v>
       </c>
       <c r="D5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3195,7 +3719,7 @@
         <v>270</v>
       </c>
       <c r="D6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3209,7 +3733,7 @@
         <v>270</v>
       </c>
       <c r="D7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3251,7 +3775,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3265,7 +3789,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3279,7 +3803,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3293,7 +3817,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4038,7 +4562,7 @@
         <v>373</v>
       </c>
       <c r="E66" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4307,7 +4831,7 @@
         <v>373</v>
       </c>
       <c r="E85" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4324,7 +4848,7 @@
         <v>373</v>
       </c>
       <c r="E86" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4341,7 +4865,7 @@
         <v>373</v>
       </c>
       <c r="E87" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4666,7 +5190,7 @@
         <v>373</v>
       </c>
       <c r="E110" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4720,50 +5244,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E47173-50DF-4235-BE7F-3CAEAD5E7694}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="3" max="3" width="95.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>387</v>
+      </c>
+      <c r="B11" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final reference fields completely analyzed.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/finals.xlsx
+++ b/analyzer/results/references/finals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC68D0BD-BD46-4F67-B613-E5CEAD7B62E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178A8A6-F781-460D-A9D3-3994D8A0B7AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="393">
   <si>
     <t>Owner</t>
   </si>
@@ -1205,6 +1205,9 @@
   </si>
   <si>
     <t>Component</t>
+  </si>
+  <si>
+    <t>Only components returned</t>
   </si>
 </sst>
 </file>
@@ -3350,7 +3353,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,7 +3362,7 @@
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="109.7109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3406,6 +3409,9 @@
       <c r="C3" t="s">
         <v>233</v>
       </c>
+      <c r="D3" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3417,6 +3423,9 @@
       <c r="C4" t="s">
         <v>188</v>
       </c>
+      <c r="D4" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -3428,6 +3437,9 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
+      <c r="D5" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3439,6 +3451,12 @@
       <c r="C6" t="s">
         <v>227</v>
       </c>
+      <c r="D6" t="s">
+        <v>392</v>
+      </c>
+      <c r="E6" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3450,6 +3468,9 @@
       <c r="C7" t="s">
         <v>77</v>
       </c>
+      <c r="D7" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3461,6 +3482,9 @@
       <c r="C8" t="s">
         <v>77</v>
       </c>
+      <c r="D8" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3472,6 +3496,9 @@
       <c r="C9" t="s">
         <v>253</v>
       </c>
+      <c r="D9" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3497,6 +3524,9 @@
       <c r="C11" t="s">
         <v>247</v>
       </c>
+      <c r="D11" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3508,6 +3538,12 @@
       <c r="C12" t="s">
         <v>259</v>
       </c>
+      <c r="D12" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3519,6 +3555,12 @@
       <c r="C13" t="s">
         <v>230</v>
       </c>
+      <c r="D13" t="s">
+        <v>378</v>
+      </c>
+      <c r="E13" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3529,6 +3571,12 @@
       </c>
       <c r="C14" t="s">
         <v>244</v>
+      </c>
+      <c r="D14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E14" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5244,10 +5292,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E47173-50DF-4235-BE7F-3CAEAD5E7694}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5330,6 +5378,11 @@
         <v>388</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Two new RuntimePermission instances added to openjdk along with methods in SecurityManager for checking those permission as well as invocations of the latter in URLConnection, Locale, and ResourceBundle.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/finals.xlsx
+++ b/analyzer/results/references/finals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EA23EC-CE17-4424-9884-2A7C11CE83AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB841AC-A5A2-44FF-80A2-353EDF81061B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="396">
   <si>
     <t>Owner</t>
   </si>
@@ -1210,17 +1210,20 @@
     <t>Only components returned</t>
   </si>
   <si>
-    <t>Should be null</t>
-  </si>
-  <si>
     <t>Internal use only</t>
+  </si>
+  <si>
+    <t>Implicitly respects tenant-isolation rules</t>
+  </si>
+  <si>
+    <t>Should be set to null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,13 +1231,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1246,13 +1273,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1533,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,16 +1598,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1615,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1596,7 +1629,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -1610,7 +1643,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -1621,13 +1654,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>373</v>
@@ -1638,41 +1671,41 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
         <v>373</v>
+      </c>
+      <c r="E7" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>373</v>
-      </c>
-      <c r="E8" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>373</v>
@@ -1680,13 +1713,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s">
         <v>373</v>
@@ -1694,13 +1727,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>373</v>
@@ -1708,7 +1741,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
@@ -1725,10 +1758,10 @@
         <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>373</v>
@@ -1739,12 +1772,15 @@
         <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
+        <v>373</v>
+      </c>
+      <c r="E14" t="s">
         <v>373</v>
       </c>
     </row>
@@ -1753,46 +1789,46 @@
         <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
         <v>373</v>
       </c>
       <c r="E15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
         <v>373</v>
-      </c>
-      <c r="E16" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
+        <v>373</v>
+      </c>
+      <c r="E17" t="s">
         <v>373</v>
       </c>
     </row>
@@ -1801,7 +1837,7 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
@@ -1815,27 +1851,24 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>373</v>
-      </c>
-      <c r="E19" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -1846,10 +1879,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -1863,7 +1896,7 @@
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
@@ -1874,13 +1907,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
         <v>373</v>
@@ -1888,33 +1921,33 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
         <v>373</v>
+      </c>
+      <c r="E24" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
         <v>373</v>
-      </c>
-      <c r="E25" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>202</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -1933,13 +1966,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
         <v>373</v>
@@ -1947,16 +1980,19 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
         <v>373</v>
+      </c>
+      <c r="E28" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1964,7 +2000,7 @@
         <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
         <v>80</v>
@@ -1978,19 +2014,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
         <v>373</v>
-      </c>
-      <c r="E30" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,10 +2031,10 @@
         <v>153</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="D31" t="s">
         <v>373</v>
@@ -2009,13 +2042,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>212</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
         <v>373</v>
@@ -2026,38 +2059,38 @@
         <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
         <v>373</v>
+      </c>
+      <c r="E33" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
         <v>373</v>
-      </c>
-      <c r="E34" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
@@ -2068,16 +2101,19 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
         <v>373</v>
+      </c>
+      <c r="E36" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,16 +2121,13 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
         <v>373</v>
-      </c>
-      <c r="E37" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,7 +2135,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>24</v>
@@ -2113,13 +2146,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
         <v>373</v>
@@ -2127,13 +2160,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
         <v>373</v>
@@ -2144,10 +2177,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D41" t="s">
         <v>373</v>
@@ -2155,44 +2188,44 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>209</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>210</v>
+        <v>111</v>
       </c>
       <c r="D42" t="s">
         <v>373</v>
+      </c>
+      <c r="E42" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
         <v>373</v>
-      </c>
-      <c r="E43" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>180</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>181</v>
       </c>
       <c r="D44" t="s">
         <v>373</v>
@@ -2200,13 +2233,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
         <v>373</v>
@@ -2214,13 +2247,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
         <v>373</v>
@@ -2228,13 +2261,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="D47" t="s">
         <v>373</v>
@@ -2242,13 +2275,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
         <v>373</v>
@@ -2259,7 +2292,7 @@
         <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
         <v>24</v>
@@ -2270,13 +2303,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
         <v>373</v>
@@ -2287,10 +2320,10 @@
         <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>373</v>
@@ -2301,10 +2334,10 @@
         <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
         <v>373</v>
@@ -2315,10 +2348,10 @@
         <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="D53" t="s">
         <v>373</v>
@@ -2326,7 +2359,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
         <v>146</v>
@@ -2340,13 +2373,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
         <v>373</v>
@@ -2354,13 +2387,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>168</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D56" t="s">
         <v>373</v>
@@ -2371,7 +2404,7 @@
         <v>168</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
         <v>21</v>
@@ -2382,13 +2415,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="D58" t="s">
         <v>373</v>
@@ -2396,13 +2429,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
         <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="D59" t="s">
         <v>373</v>
@@ -2410,13 +2443,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="D60" t="s">
         <v>373</v>
@@ -2424,13 +2457,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
         <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
         <v>373</v>
@@ -2438,13 +2471,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
         <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
         <v>373</v>
@@ -2452,13 +2485,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
         <v>373</v>
@@ -2466,13 +2499,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
         <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D64" t="s">
         <v>373</v>
@@ -2480,13 +2513,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
         <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="D65" t="s">
         <v>373</v>
@@ -2494,13 +2527,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="B66" t="s">
         <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="D66" t="s">
         <v>373</v>
@@ -2508,13 +2541,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="B67" t="s">
         <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="D67" t="s">
         <v>373</v>
@@ -2522,21 +2555,21 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
         <v>14</v>
@@ -2550,7 +2583,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="B70" t="s">
         <v>14</v>
@@ -2564,13 +2597,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
         <v>372</v>
@@ -2581,7 +2614,7 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
         <v>18</v>
@@ -2592,13 +2625,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
       <c r="D73" t="s">
         <v>372</v>
@@ -2606,13 +2639,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>208</v>
       </c>
       <c r="C74" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="D74" t="s">
         <v>372</v>
@@ -2620,13 +2653,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>207</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>208</v>
+        <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>207</v>
+        <v>15</v>
       </c>
       <c r="D75" t="s">
         <v>372</v>
@@ -2634,13 +2667,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D76" t="s">
         <v>372</v>
@@ -2648,13 +2681,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D77" t="s">
         <v>372</v>
@@ -2662,13 +2695,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D78" t="s">
         <v>372</v>
@@ -2676,7 +2709,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="B79" t="s">
         <v>102</v>
@@ -2690,13 +2723,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>71</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D80" t="s">
         <v>372</v>
@@ -2707,7 +2740,7 @@
         <v>71</v>
       </c>
       <c r="B81" t="s">
-        <v>72</v>
+        <v>203</v>
       </c>
       <c r="C81" t="s">
         <v>73</v>
@@ -2718,13 +2751,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D82" t="s">
         <v>372</v>
@@ -2732,13 +2765,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="D83" t="s">
         <v>372</v>
@@ -2746,13 +2779,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>213</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>213</v>
       </c>
       <c r="D84" t="s">
         <v>372</v>
@@ -2760,13 +2793,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="B85" t="s">
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="D85" t="s">
         <v>372</v>
@@ -2774,13 +2807,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>187</v>
+        <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="D86" t="s">
         <v>372</v>
@@ -2788,10 +2821,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B87" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
@@ -2802,13 +2835,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="C88" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D88" t="s">
         <v>372</v>
@@ -2816,13 +2849,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>33</v>
+        <v>223</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="C89" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D89" t="s">
         <v>372</v>
@@ -2830,10 +2863,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C90" t="s">
         <v>15</v>
@@ -2844,13 +2877,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="D91" t="s">
         <v>372</v>
@@ -2858,58 +2891,61 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C92" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D92" t="s">
-        <v>372</v>
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="B93" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="D93" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="B94" t="s">
-        <v>87</v>
+        <v>166</v>
       </c>
       <c r="C94" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
       <c r="D94" t="s">
-        <v>375</v>
+        <v>393</v>
+      </c>
+      <c r="E94" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="D95" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
       <c r="E95" t="s">
         <v>372</v>
@@ -2917,58 +2953,67 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>221</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>222</v>
       </c>
       <c r="D96" t="s">
-        <v>375</v>
+        <v>393</v>
+      </c>
+      <c r="E96" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>144</v>
+        <v>57</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D97" t="s">
-        <v>375</v>
+        <v>393</v>
+      </c>
+      <c r="E97" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C98" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>375</v>
+        <v>393</v>
+      </c>
+      <c r="E98" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="B99" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="C99" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D99" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
       <c r="E99" t="s">
         <v>372</v>
@@ -2976,61 +3021,61 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>188</v>
+        <v>90</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>91</v>
       </c>
       <c r="C100" t="s">
-        <v>190</v>
+        <v>92</v>
       </c>
       <c r="D100" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B101" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="C101" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
-        <v>378</v>
-      </c>
-      <c r="E101" t="s">
-        <v>372</v>
+        <v>393</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>75</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>76</v>
       </c>
       <c r="C102" t="s">
-        <v>206</v>
+        <v>77</v>
       </c>
       <c r="D102" t="s">
-        <v>378</v>
+        <v>393</v>
+      </c>
+      <c r="E102" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>22</v>
+        <v>199</v>
       </c>
       <c r="B103" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="C103" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="D103" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
       <c r="E103" t="s">
         <v>372</v>
@@ -3038,225 +3083,210 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>197</v>
+        <v>101</v>
       </c>
       <c r="C104" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D104" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
       <c r="E104" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>217</v>
       </c>
       <c r="C105" t="s">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="D105" t="s">
-        <v>378</v>
-      </c>
-      <c r="E105" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C106" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D106" t="s">
-        <v>378</v>
-      </c>
-      <c r="E106" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
       <c r="B107" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="C107" t="s">
-        <v>86</v>
-      </c>
-      <c r="D107" t="s">
-        <v>389</v>
+        <v>125</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="B108" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="C108" t="s">
-        <v>167</v>
-      </c>
-      <c r="D108" t="s">
-        <v>389</v>
-      </c>
-      <c r="E108" t="s">
-        <v>372</v>
+        <v>88</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="B109" t="s">
-        <v>221</v>
+        <v>97</v>
       </c>
       <c r="C109" t="s">
-        <v>222</v>
-      </c>
-      <c r="D109" t="s">
-        <v>389</v>
+        <v>98</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>375</v>
       </c>
       <c r="E109" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B110" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C110" t="s">
-        <v>92</v>
-      </c>
-      <c r="D110" t="s">
-        <v>389</v>
+        <v>61</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
-      </c>
-      <c r="D111" t="s">
-        <v>389</v>
+        <v>61</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="B112" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="C112" t="s">
-        <v>201</v>
-      </c>
-      <c r="D112" t="s">
-        <v>389</v>
-      </c>
-      <c r="E112" t="s">
-        <v>372</v>
+        <v>173</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="C113" t="s">
-        <v>77</v>
-      </c>
-      <c r="D113" t="s">
-        <v>381</v>
+        <v>136</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>375</v>
       </c>
       <c r="E113" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>188</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
+        <v>189</v>
       </c>
       <c r="C114" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="D114" t="s">
-        <v>381</v>
-      </c>
-      <c r="E114" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>216</v>
+        <v>52</v>
       </c>
       <c r="B115" t="s">
-        <v>217</v>
+        <v>53</v>
       </c>
       <c r="C115" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
       <c r="D115" t="s">
-        <v>381</v>
+        <v>378</v>
+      </c>
+      <c r="E115" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>38</v>
+        <v>204</v>
       </c>
       <c r="B116" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="C116" t="s">
-        <v>40</v>
+        <v>206</v>
       </c>
       <c r="D116" t="s">
-        <v>394</v>
-      </c>
-      <c r="E116" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B117" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
       <c r="C117" t="s">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="D117" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="E117" t="s">
         <v>372</v>
@@ -3264,16 +3294,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="B118" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C118" t="s">
-        <v>178</v>
+        <v>54</v>
       </c>
       <c r="D118" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="E118" t="s">
         <v>372</v>
@@ -3281,33 +3311,36 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="C119" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="D119" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="E119" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>387</v>
+        <v>378</v>
+      </c>
+      <c r="E120" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3320,7 +3353,7 @@
       <c r="C121" t="s">
         <v>193</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="2" t="s">
         <v>377</v>
       </c>
       <c r="E121" t="s">
@@ -3335,24 +3368,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF6BABD1-A540-4C4E-B17D-ADDB27355019}">
-          <x14:formula1>
-            <xm:f>reasons!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A7D80AD-B76D-4F4E-808A-082975E23528}">
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D21 D25:D27 D29:D40 D68:D115 D120</xm:sqref>
+          <xm:sqref>D3:D21 D25:D27 D29:D40 D120 D68:D110</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88E6E823-CE9D-4823-8F74-575665822849}">
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D121:E121 E2:E21 D22:E24 D28 E25:E120 D41:D67 D116:D119</xm:sqref>
+          <xm:sqref>D121:E121 E2:E21 D22:E24 D28 E25:E120 D41:D67 D2 D111:D119</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3365,7 +3392,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3598,16 +3625,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D16" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
       <c r="E16" t="s">
         <v>372</v>
@@ -3615,36 +3642,36 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="D17" t="s">
         <v>378</v>
       </c>
       <c r="E17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="D18" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="E18" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3684,8 +3711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3600B5-2A22-43DF-8B3A-881817398BDB}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5209,8 +5236,8 @@
       <c r="C107" t="s">
         <v>303</v>
       </c>
-      <c r="D107" t="s">
-        <v>393</v>
+      <c r="D107" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -5223,8 +5250,8 @@
       <c r="C108" t="s">
         <v>344</v>
       </c>
-      <c r="D108" t="s">
-        <v>393</v>
+      <c r="D108" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,7 +5264,7 @@
       <c r="C109" t="s">
         <v>303</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -5251,7 +5278,7 @@
       <c r="C110" t="s">
         <v>303</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -5265,7 +5292,7 @@
       <c r="C111" t="s">
         <v>270</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -5279,7 +5306,7 @@
       <c r="C112" t="s">
         <v>270</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -5295,13 +5322,13 @@
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E112 D6:D112 D2 D4</xm:sqref>
+          <xm:sqref>E2:E112 D4 D2 D6:D106 D109:D112</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{817C4072-F7D0-42A1-AC68-86BED1530349}">
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D5 D3</xm:sqref>
+          <xm:sqref>D5 D3 D107:D108</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5311,10 +5338,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E47173-50DF-4235-BE7F-3CAEAD5E7694}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5404,11 +5431,16 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>394</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fix regarding new permission checks in OpenJDK source.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/finals.xlsx
+++ b/analyzer/results/references/finals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB841AC-A5A2-44FF-80A2-353EDF81061B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C781CA-46C4-4CF5-9DEE-4AFEC6980676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId1"/>
@@ -1192,12 +1192,6 @@
     <t>This shouldn't be used</t>
   </si>
   <si>
-    <t>ThreadLocal</t>
-  </si>
-  <si>
-    <t>Since each thread belongs to one and only one tenant at any given time, changes in static ThreadLocal variables do not violate tenant-isolation requirements</t>
-  </si>
-  <si>
     <t>Never returned</t>
   </si>
   <si>
@@ -1217,6 +1211,12 @@
   </si>
   <si>
     <t>Should be set to null</t>
+  </si>
+  <si>
+    <t>Irrelevant</t>
+  </si>
+  <si>
+    <t>For instance, it's never useful on server-side</t>
   </si>
 </sst>
 </file>
@@ -1233,14 +1233,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1255,12 +1255,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1280,12 +1280,12 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1566,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,52 +2900,52 @@
         <v>123</v>
       </c>
       <c r="D92" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="C93" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="D93" t="s">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="E93" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="B94" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C94" t="s">
-        <v>167</v>
+        <v>86</v>
       </c>
       <c r="D94" t="s">
-        <v>393</v>
-      </c>
-      <c r="E94" t="s">
-        <v>372</v>
+        <v>391</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="C95" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="D95" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E95" t="s">
         <v>372</v>
@@ -2962,7 +2962,7 @@
         <v>222</v>
       </c>
       <c r="D96" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E96" t="s">
         <v>373</v>
@@ -2979,7 +2979,7 @@
         <v>65</v>
       </c>
       <c r="D97" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E97" t="s">
         <v>372</v>
@@ -2996,7 +2996,7 @@
         <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E98" t="s">
         <v>372</v>
@@ -3013,7 +3013,7 @@
         <v>158</v>
       </c>
       <c r="D99" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E99" t="s">
         <v>372</v>
@@ -3030,7 +3030,7 @@
         <v>92</v>
       </c>
       <c r="D100" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>114</v>
       </c>
       <c r="D101" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
         <v>77</v>
       </c>
       <c r="D102" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E102" t="s">
         <v>381</v>
@@ -3075,7 +3075,7 @@
         <v>201</v>
       </c>
       <c r="D103" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E103" t="s">
         <v>372</v>
@@ -3092,7 +3092,7 @@
         <v>77</v>
       </c>
       <c r="D104" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E104" t="s">
         <v>381</v>
@@ -3109,7 +3109,7 @@
         <v>218</v>
       </c>
       <c r="D105" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
         <v>58</v>
       </c>
       <c r="D106" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3345,13 +3345,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B121" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="C121" t="s">
-        <v>193</v>
+        <v>40</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>377</v>
@@ -3418,7 +3418,7 @@
         <v>384</v>
       </c>
       <c r="E1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
         <v>227</v>
       </c>
       <c r="D16" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E16" t="s">
         <v>372</v>
@@ -3711,8 +3711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3600B5-2A22-43DF-8B3A-881817398BDB}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5237,7 +5237,7 @@
         <v>303</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,7 +5251,7 @@
         <v>344</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5340,8 +5340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E47173-50DF-4235-BE7F-3CAEAD5E7694}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5369,7 +5369,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5398,7 +5398,7 @@
         <v>377</v>
       </c>
       <c r="B7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5418,30 +5418,30 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="B11" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Field analysis results updated.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/finals.xlsx
+++ b/analyzer/results/references/finals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AB690E-2B84-49EB-BAD5-EE0AF98440F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA31D3A5-2BCE-40DD-A38D-4504F4395EBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -931,9 +931,6 @@
     <t>Field type is not immutable but the assigned values to the final field are immutable</t>
   </si>
   <si>
-    <t>Never returned to tenant modules</t>
-  </si>
-  <si>
     <t>For instance, the type is not a final class and can be subclassed but it is not subclassed in java.base and not exported to tenant modules</t>
   </si>
   <si>
@@ -974,6 +971,9 @@
   </si>
   <si>
     <t>For instance, it's never useful on server-side</t>
+  </si>
+  <si>
+    <t>Effectively immutable final</t>
   </si>
 </sst>
 </file>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D90" activeCellId="1" sqref="D89 D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,10 +1347,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" t="s">
         <v>303</v>
-      </c>
-      <c r="E1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
         <v>107</v>
       </c>
       <c r="D71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
         <v>174</v>
       </c>
       <c r="D72" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E72" t="s">
         <v>291</v>
@@ -2394,7 +2394,7 @@
         <v>71</v>
       </c>
       <c r="D73" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>149</v>
       </c>
       <c r="D74" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E74" t="s">
         <v>291</v>
@@ -2425,7 +2425,7 @@
         <v>199</v>
       </c>
       <c r="D75" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E75" t="s">
         <v>292</v>
@@ -2442,7 +2442,7 @@
         <v>53</v>
       </c>
       <c r="D76" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E76" t="s">
         <v>291</v>
@@ -2459,7 +2459,7 @@
         <v>160</v>
       </c>
       <c r="D77" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E77" t="s">
         <v>291</v>
@@ -2476,7 +2476,7 @@
         <v>140</v>
       </c>
       <c r="D78" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E78" t="s">
         <v>291</v>
@@ -2493,7 +2493,7 @@
         <v>77</v>
       </c>
       <c r="D79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
         <v>98</v>
       </c>
       <c r="D80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2521,10 +2521,10 @@
         <v>62</v>
       </c>
       <c r="D81" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E81" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
         <v>181</v>
       </c>
       <c r="D82" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E82" t="s">
         <v>291</v>
@@ -2555,10 +2555,10 @@
         <v>62</v>
       </c>
       <c r="D83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E83" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
         <v>195</v>
       </c>
       <c r="D84" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
         <v>48</v>
       </c>
       <c r="D85" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2599,8 +2599,8 @@
       <c r="C86" t="s">
         <v>109</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>294</v>
+      <c r="D86" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2613,8 +2613,8 @@
       <c r="C87" t="s">
         <v>73</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>294</v>
+      <c r="D87" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,8 +2644,8 @@
       <c r="C89" t="s">
         <v>49</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>294</v>
+      <c r="D89" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,8 +2658,8 @@
       <c r="C90" t="s">
         <v>49</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>294</v>
+      <c r="D90" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2672,8 +2672,8 @@
       <c r="C91" t="s">
         <v>155</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>294</v>
+      <c r="D91" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2686,8 +2686,8 @@
       <c r="C92" t="s">
         <v>118</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>294</v>
+      <c r="D92" t="s">
+        <v>309</v>
       </c>
       <c r="E92" t="s">
         <v>291</v>
@@ -2842,7 +2842,7 @@
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D100:E100 E3:E22 D23:E25 D29 D42:D68 D3 D91:D99 E1 E26:E99</xm:sqref>
+          <xm:sqref>D100:E100 E3:E22 D23:E25 D29 D42:D68 D3 E26:E99 E1 D92:D99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2855,7 +2855,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,10 +2878,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,7 +2926,7 @@
         <v>292</v>
       </c>
       <c r="E4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3069,7 +3069,7 @@
         <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E14" t="s">
         <v>291</v>
@@ -3146,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3600B5-2A22-43DF-8B3A-881817398BDB}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,10 +3170,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" t="s">
         <v>303</v>
-      </c>
-      <c r="E1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3803,7 +3803,7 @@
       <c r="C45" t="s">
         <v>257</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       <c r="C46" t="s">
         <v>278</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3861,13 +3861,13 @@
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D4 D2 D6:D48 E2:E48</xm:sqref>
+          <xm:sqref>D4 D2 E2:E48 D6:D44 D47:D48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{817C4072-F7D0-42A1-AC68-86BED1530349}">
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D5 D3</xm:sqref>
+          <xm:sqref>D5 D3 D45:D46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3880,7 +3880,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,12 +3903,12 @@
         <v>299</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,7 +3937,7 @@
         <v>296</v>
       </c>
       <c r="B7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3947,40 +3947,40 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" t="s">
         <v>313</v>
-      </c>
-      <c r="B11" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>